<commit_message>
Tested submit multiple choices for checkbox.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21903"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F87CEE7-ACC9-45E8-9AAF-B81DD7897F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{1F87CEE7-ACC9-45E8-9AAF-B81DD7897F1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4C50A5B2-302C-42B5-90A8-6FBDABD0F96C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>华语网辩报名信息</t>
   </si>
@@ -35,16 +36,19 @@
     <t>测试链接</t>
   </si>
   <si>
-    <t>测试开始日期</t>
-  </si>
-  <si>
-    <t>测试结束日期</t>
+    <t>测试开始时间</t>
+  </si>
+  <si>
+    <t>测试结束时间</t>
   </si>
   <si>
     <t>正式链接</t>
   </si>
   <si>
-    <t>报名开始日期</t>
+    <t>开始填表时间</t>
+  </si>
+  <si>
+    <t>报名开始时间</t>
   </si>
   <si>
     <t>队伍名称</t>
@@ -65,6 +69,12 @@
     <t>https://www.wjx.cn/jq/42426112.aspx</t>
   </si>
   <si>
+    <t>2019-07-07 07:30</t>
+  </si>
+  <si>
+    <t>2019-07-07 08:00</t>
+  </si>
+  <si>
     <t>特别乐群队</t>
   </si>
   <si>
@@ -159,16 +169,13 @@
   </si>
   <si>
     <t>二等奖卡山谷，和女警看来你，家开的不能刷卡</t>
-  </si>
-  <si>
-    <t>2019-07-05 22:39</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +215,11 @@
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -241,6 +253,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,30 +535,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="35.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -567,28 +581,34 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -609,7 +629,7 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
@@ -621,9 +641,9 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -635,131 +655,131 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="18">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2" t="s">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +795,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -783,40 +803,40 @@
     <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="18">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>

</xml_diff>

<commit_message>
Added submit time waiting
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21903"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{1F87CEE7-ACC9-45E8-9AAF-B81DD7897F1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4C50A5B2-302C-42B5-90A8-6FBDABD0F96C}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{1F87CEE7-ACC9-45E8-9AAF-B81DD7897F1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FF7F1916-CE9E-4740-8AB1-934D0CC9F7D8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>华语网辩报名信息</t>
   </si>
@@ -57,22 +57,19 @@
     <t>比赛项目</t>
   </si>
   <si>
-    <t>https://www.wjx.cn/jq/42413695.aspx</t>
-  </si>
-  <si>
-    <t>2019-07-03  00:01</t>
-  </si>
-  <si>
-    <t>2019-07-05  10:00</t>
-  </si>
-  <si>
-    <t>https://www.wjx.cn/jq/42426112.aspx</t>
-  </si>
-  <si>
-    <t>2019-07-07 07:30</t>
-  </si>
-  <si>
-    <t>2019-07-07 08:00</t>
+    <t>https://www.wjx.cn/jq/42340427.aspx</t>
+  </si>
+  <si>
+    <t>2019-07-03  00:01:00</t>
+  </si>
+  <si>
+    <t>2019-07-07  16:53:00</t>
+  </si>
+  <si>
+    <t>2019-07-07 16:53:00</t>
+  </si>
+  <si>
+    <t>2019-07-07 16:55:00</t>
   </si>
   <si>
     <t>特别乐群队</t>
@@ -153,6 +150,9 @@
     <t>评委姓名</t>
   </si>
   <si>
+    <t>评委本科入学年份</t>
+  </si>
+  <si>
     <t>评委QQ</t>
   </si>
   <si>
@@ -162,13 +162,19 @@
     <t>评委履历</t>
   </si>
   <si>
-    <t>小白</t>
-  </si>
-  <si>
-    <t>1425053301</t>
-  </si>
-  <si>
-    <t>二等奖卡山谷，和女警看来你，家开的不能刷卡</t>
+    <t>高子柳</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>1010678911</t>
+  </si>
+  <si>
+    <t>13880551583</t>
+  </si>
+  <si>
+    <t>很厉害，超厉害</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -595,29 +601,26 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{F1CC1544-E432-45F7-90CC-2580DA036DE9}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{EA0ABA4F-FA2B-4AA7-92E9-1C5AC993B76D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -643,7 +646,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -657,129 +660,129 @@
     </row>
     <row r="2" spans="1:10" ht="18">
       <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -792,20 +795,21 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="7"/>
+    <col min="5" max="5" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -813,15 +817,18 @@
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -833,12 +840,14 @@
         <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="F3" s="6"/>
     </row>
   </sheetData>

</xml_diff>